<commit_message>
Add a Robot Model dialog now fully functioning
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinton\Documents\Visual Studio 2015\Projects\HW6\Homework_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinton\Documents\Visual Studio 2015\Projects\HW6\HW6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="627" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="627" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,16 @@
     <sheet name="Sprint 3 Backlog" sheetId="5" r:id="rId4"/>
     <sheet name="Sprint 4 Backlog" sheetId="6" r:id="rId5"/>
     <sheet name="Sprint 5 Backlog" sheetId="7" r:id="rId6"/>
-    <sheet name="Sprint NN Backlog" sheetId="2" r:id="rId7"/>
+    <sheet name="Sprint 6 Backlog" sheetId="8" r:id="rId7"/>
+    <sheet name="Sprint 7 Backlog" sheetId="9" r:id="rId8"/>
+    <sheet name="Sprint NN Backlog" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="289">
   <si>
     <t>Product Name:</t>
   </si>
@@ -809,42 +811,12 @@
     <t>Add necessary code to display window and run FLTK</t>
   </si>
   <si>
-    <t>Also comment out the CLI portion of code</t>
-  </si>
-  <si>
-    <t>Add Fl_Menu_Bar</t>
-  </si>
-  <si>
-    <t>Add a "Create" option to the menu bar with a submenu option for Robot_Part</t>
-  </si>
-  <si>
-    <t>Add Fl_input dialogs that will ask user for information for creating a Robot_Part</t>
-  </si>
-  <si>
-    <t>Add callback to that option that will call Controller's input dialogs</t>
-  </si>
-  <si>
     <t>Makefile</t>
   </si>
   <si>
-    <t>Add Fl_input dialogs that will ask user for information for creating a Robot_Model</t>
-  </si>
-  <si>
-    <t>Update Menu_Bar to also have a option for Robot_Models</t>
-  </si>
-  <si>
-    <t>Add submenu option under Create</t>
-  </si>
-  <si>
     <t>Create new Makefile to correctly compile a FLTK program</t>
   </si>
   <si>
-    <t>Update Makefile with Controller</t>
-  </si>
-  <si>
-    <t>Add Controller</t>
-  </si>
-  <si>
     <t>Backup</t>
   </si>
   <si>
@@ -852,6 +824,78 @@
   </si>
   <si>
     <t>Set up git repository for Homework 6</t>
+  </si>
+  <si>
+    <t>Get FLTK to correctly compile on machine</t>
+  </si>
+  <si>
+    <t>Create a menu bar</t>
+  </si>
+  <si>
+    <t>Create a menu bar item with a submenu option to create a robot part</t>
+  </si>
+  <si>
+    <t>Menu title: "Create"; Submenu title: "Robot Part"</t>
+  </si>
+  <si>
+    <t>Create a callback for Create&gt;Robot Part that calls aforementioned dialog</t>
+  </si>
+  <si>
+    <t>Update Makefile as needed</t>
+  </si>
+  <si>
+    <t>Create new submenu option under Create for a Robot Model</t>
+  </si>
+  <si>
+    <t>Create a function that will call Fl_input dialogs to collect robot model info</t>
+  </si>
+  <si>
+    <t>Create a callback for Create&gt;Robot Model that calls aforementioned dialog</t>
+  </si>
+  <si>
+    <t>6 &amp; 7</t>
+  </si>
+  <si>
+    <t>Create a class that will call Fl_input dialogs to collect robot part info</t>
+  </si>
+  <si>
+    <t>Create a class that will call Fl_input dialogs to collect robot model info</t>
+  </si>
+  <si>
+    <t>Create a class that will output current robot model info</t>
+  </si>
+  <si>
+    <t>Menu option: Report &gt; All Robot Models</t>
+  </si>
+  <si>
+    <t>Update Create Robot Model dialog to also include adding a picture</t>
+  </si>
+  <si>
+    <t>Update Makefile for compiling pictures</t>
+  </si>
+  <si>
+    <t>Update Robot Model List dialog to display the previously chosen picture</t>
+  </si>
+  <si>
+    <t>Add menu option for listing robot models</t>
+  </si>
+  <si>
+    <t>Add methods for extracting information</t>
+  </si>
+  <si>
+    <t>Design callbacks for widgets in listing class</t>
+  </si>
+  <si>
+    <t>Update UML diagrams</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Create debug option to generate random robot parts</t>
+  </si>
+  <si>
+    <t>Create debug option to generate random robot models</t>
   </si>
 </sst>
 </file>
@@ -1262,16 +1306,16 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3146,7 +3190,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sprint 5 Backlog'!$A$57:$A$64</c:f>
+              <c:f>'Sprint 5 Backlog'!$A$48:$A$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3179,33 +3223,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sprint 5 Backlog'!$B$57:$B$64</c:f>
+              <c:f>'Sprint 5 Backlog'!$B$48:$B$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3470,6 +3514,826 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 6 Burn</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sprint 6 Backlog'!$A$48:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sprint 6 Backlog'!$B$48:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2BFE-4D83-BCD7-829E6DBD7B5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="393249400"/>
+        <c:axId val="1"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="393249400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Left</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393249400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 7 Burn</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sprint 7 Backlog'!$A$48:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sprint 7 Backlog'!$B$48:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC90-411A-A3AE-4A9157D6083D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="393249400"/>
+        <c:axId val="1"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="393249400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Calibri"/>
+                <a:cs typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Left</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="393249400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3935,6 +4799,80 @@
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -4268,8 +5206,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4627,8 +5565,8 @@
         <v>15</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>B25-1</f>
+        <v>31</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>14</v>
@@ -4648,7 +5586,7 @@
       </c>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>14</v>
@@ -4668,7 +5606,7 @@
       </c>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>14</v>
@@ -4688,7 +5626,7 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>14</v>
@@ -4772,7 +5710,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D34" s="42">
         <v>5</v>
@@ -4830,10 +5768,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="D36" s="39">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -4888,10 +5826,10 @@
         <v>5</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="D38" s="39">
-        <v>5</v>
+        <v>154</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>274</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -4949,7 +5887,7 @@
         <v>148</v>
       </c>
       <c r="D40" s="42">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -4978,7 +5916,7 @@
         <v>148</v>
       </c>
       <c r="D41" s="42">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -5036,7 +5974,7 @@
         <v>148</v>
       </c>
       <c r="D43" s="42">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -5065,7 +6003,7 @@
         <v>148</v>
       </c>
       <c r="D44" s="42">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -5094,7 +6032,7 @@
         <v>148</v>
       </c>
       <c r="D45" s="42">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -8221,10 +9159,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8309,8 +9247,8 @@
         <v>135</v>
       </c>
       <c r="B6" s="35">
-        <f>COUNT(A21:A50)</f>
-        <v>16</v>
+        <f>COUNT(A21:A41)</f>
+        <v>8</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
@@ -8325,7 +9263,7 @@
       </c>
       <c r="B7" s="35">
         <f>SUM(B6)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -8340,7 +9278,7 @@
       </c>
       <c r="B8" s="35">
         <f>SUM(B7)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -8355,7 +9293,7 @@
       </c>
       <c r="B9" s="35">
         <f>SUM(B8, -1)</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -8369,8 +9307,8 @@
         <v>139</v>
       </c>
       <c r="B10" s="35">
-        <f>SUM(B9)</f>
-        <v>15</v>
+        <f>SUM(B9, -2)</f>
+        <v>5</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -8384,8 +9322,8 @@
         <v>140</v>
       </c>
       <c r="B11" s="35">
-        <f>SUM(B10)</f>
-        <v>15</v>
+        <f>SUM(B10, -1)</f>
+        <v>4</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -8399,8 +9337,8 @@
         <v>141</v>
       </c>
       <c r="B12" s="35">
-        <f>SUM(B11)</f>
-        <v>15</v>
+        <f>SUM(B11, -4)</f>
+        <v>0</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -8415,7 +9353,7 @@
       </c>
       <c r="B13" s="35">
         <f>SUM(B12)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -8494,19 +9432,19 @@
         <v>160</v>
       </c>
       <c r="C22" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D22" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="E22" t="s">
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -8529,7 +9467,7 @@
         <v>258</v>
       </c>
       <c r="G23" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -8552,7 +9490,7 @@
         <v>256</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -8575,7 +9513,7 @@
         <v>257</v>
       </c>
       <c r="G25" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -8598,7 +9536,7 @@
         <v>259</v>
       </c>
       <c r="G26" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -8612,16 +9550,16 @@
         <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E27" t="s">
         <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="G27" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -8629,284 +9567,94 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>247</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="E28" t="s">
         <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G28" t="s">
-        <v>148</v>
-      </c>
-      <c r="H28" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ref="B48:B55" si="0">B6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B29" t="s">
-        <v>216</v>
-      </c>
-      <c r="C29" t="s">
-        <v>152</v>
-      </c>
-      <c r="D29" t="s">
-        <v>255</v>
-      </c>
-      <c r="E29" t="s">
-        <v>150</v>
-      </c>
-      <c r="F29" t="s">
-        <v>271</v>
-      </c>
-      <c r="G29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>216</v>
-      </c>
-      <c r="C30" t="s">
-        <v>152</v>
-      </c>
-      <c r="D30" t="s">
-        <v>255</v>
-      </c>
-      <c r="E30" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" t="s">
-        <v>261</v>
-      </c>
-      <c r="G30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>9</v>
-      </c>
-      <c r="B31" t="s">
-        <v>216</v>
-      </c>
-      <c r="C31" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" t="s">
-        <v>255</v>
-      </c>
-      <c r="E31" t="s">
-        <v>150</v>
-      </c>
-      <c r="F31" t="s">
-        <v>262</v>
-      </c>
-      <c r="G31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>10</v>
-      </c>
-      <c r="B32" t="s">
-        <v>216</v>
-      </c>
-      <c r="C32" t="s">
-        <v>152</v>
-      </c>
-      <c r="D32" t="s">
-        <v>255</v>
-      </c>
-      <c r="E32" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32" t="s">
-        <v>264</v>
-      </c>
-      <c r="G32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" t="s">
-        <v>152</v>
-      </c>
-      <c r="D33" t="s">
-        <v>265</v>
-      </c>
-      <c r="E33" t="s">
-        <v>150</v>
-      </c>
-      <c r="F33" t="s">
-        <v>270</v>
-      </c>
-      <c r="G33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E34" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" t="s">
-        <v>266</v>
-      </c>
-      <c r="G34" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>13</v>
-      </c>
-      <c r="B35" t="s">
-        <v>217</v>
-      </c>
-      <c r="C35" t="s">
-        <v>152</v>
-      </c>
-      <c r="D35" t="s">
-        <v>255</v>
-      </c>
-      <c r="E35" t="s">
-        <v>150</v>
-      </c>
-      <c r="F35" t="s">
-        <v>267</v>
-      </c>
-      <c r="G35" t="s">
-        <v>148</v>
-      </c>
-      <c r="H35" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>14</v>
-      </c>
-      <c r="B36" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" t="s">
-        <v>152</v>
-      </c>
-      <c r="D36" t="s">
-        <v>255</v>
-      </c>
-      <c r="E36" t="s">
-        <v>150</v>
-      </c>
-      <c r="F36" t="s">
-        <v>264</v>
-      </c>
-      <c r="G36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B57">
-        <f t="shared" ref="B57:B64" si="0">B6</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>2</v>
-      </c>
-      <c r="B59">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>3</v>
-      </c>
-      <c r="B60">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>4</v>
-      </c>
-      <c r="B61">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>5</v>
-      </c>
-      <c r="B62">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>6</v>
-      </c>
-      <c r="B63">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>7</v>
-      </c>
-      <c r="B64">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8920,6 +9668,1112 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="32">
+        <v>6</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="33">
+        <v>42677.333333333336</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="33">
+        <v>42684.333333333336</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="34">
+        <f>B3</f>
+        <v>42684.333333333336</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="35">
+        <f>COUNT(A21:A45)</f>
+        <v>9</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="35">
+        <f>SUM(B6)</f>
+        <v>9</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="35">
+        <f>SUM(B7, -3)</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="35">
+        <f>SUM(B8)</f>
+        <v>6</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="35">
+        <f>SUM(B9)</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="35">
+        <f>SUM(B10, -3)</f>
+        <v>3</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="35">
+        <f>SUM(B11)</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="35">
+        <f>SUM(B12, -2)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" t="s">
+        <v>255</v>
+      </c>
+      <c r="E21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" t="s">
+        <v>266</v>
+      </c>
+      <c r="G21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" t="s">
+        <v>267</v>
+      </c>
+      <c r="G22" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
+        <v>269</v>
+      </c>
+      <c r="G24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" t="s">
+        <v>270</v>
+      </c>
+      <c r="G25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>255</v>
+      </c>
+      <c r="E26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" t="s">
+        <v>271</v>
+      </c>
+      <c r="G26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" t="s">
+        <v>272</v>
+      </c>
+      <c r="G27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>255</v>
+      </c>
+      <c r="E28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" t="s">
+        <v>273</v>
+      </c>
+      <c r="G28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D29" t="s">
+        <v>260</v>
+      </c>
+      <c r="E29" t="s">
+        <v>150</v>
+      </c>
+      <c r="F29" t="s">
+        <v>270</v>
+      </c>
+      <c r="G29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ref="B48:B55" si="0">B6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="32">
+        <v>7</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="33">
+        <v>42684.333333333336</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="33">
+        <v>42691.333333333336</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="34">
+        <f>B3</f>
+        <v>42691.333333333336</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="35">
+        <f>COUNT(A21:A45)</f>
+        <v>11</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="35">
+        <f>SUM(B6)</f>
+        <v>11</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="35">
+        <f>SUM(B7)</f>
+        <v>11</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="35">
+        <f>SUM(B8)</f>
+        <v>11</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="35">
+        <f>SUM(B9)</f>
+        <v>11</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="35">
+        <f>SUM(B10)</f>
+        <v>11</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="35">
+        <f>SUM(B11)</f>
+        <v>11</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="35">
+        <f>SUM(B12)</f>
+        <v>11</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" t="s">
+        <v>255</v>
+      </c>
+      <c r="E21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" t="s">
+        <v>276</v>
+      </c>
+      <c r="G21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" t="s">
+        <v>277</v>
+      </c>
+      <c r="G22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" t="s">
+        <v>255</v>
+      </c>
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" t="s">
+        <v>283</v>
+      </c>
+      <c r="G23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" t="s">
+        <v>284</v>
+      </c>
+      <c r="G24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>255</v>
+      </c>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" t="s">
+        <v>282</v>
+      </c>
+      <c r="G25" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>219</v>
+      </c>
+      <c r="C26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" t="s">
+        <v>255</v>
+      </c>
+      <c r="E26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" t="s">
+        <v>279</v>
+      </c>
+      <c r="G26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" t="s">
+        <v>260</v>
+      </c>
+      <c r="E27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" t="s">
+        <v>280</v>
+      </c>
+      <c r="G27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>255</v>
+      </c>
+      <c r="E28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" t="s">
+        <v>281</v>
+      </c>
+      <c r="G28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" t="s">
+        <v>150</v>
+      </c>
+      <c r="F29" t="s">
+        <v>285</v>
+      </c>
+      <c r="G29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" t="s">
+        <v>286</v>
+      </c>
+      <c r="E30" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" t="s">
+        <v>287</v>
+      </c>
+      <c r="G30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" t="s">
+        <v>286</v>
+      </c>
+      <c r="E31" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" t="s">
+        <v>288</v>
+      </c>
+      <c r="G31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ref="B48:B55" si="0">B6</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H15"/>

</xml_diff>

<commit_message>
started List Robot Models dialog
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -1309,13 +1309,13 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4051,25 +4051,25 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5206,8 +5206,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5585,8 +5585,8 @@
         <v>16</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f>B26-1</f>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>14</v>
@@ -5605,8 +5605,8 @@
         <v>17</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f>B27-1</f>
+        <v>29</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>14</v>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>14</v>
@@ -5826,7 +5826,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D38" s="39" t="s">
         <v>274</v>
@@ -5884,7 +5884,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D40" s="42">
         <v>7</v>
@@ -10202,7 +10202,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10302,8 +10302,8 @@
         <v>136</v>
       </c>
       <c r="B7" s="35">
-        <f>SUM(B6)</f>
-        <v>11</v>
+        <f>SUM(B6, -2)</f>
+        <v>9</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -10317,8 +10317,8 @@
         <v>137</v>
       </c>
       <c r="B8" s="35">
-        <f>SUM(B7)</f>
-        <v>11</v>
+        <f>SUM(B7, -2)</f>
+        <v>7</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -10332,8 +10332,8 @@
         <v>138</v>
       </c>
       <c r="B9" s="35">
-        <f>SUM(B8)</f>
-        <v>11</v>
+        <f t="shared" ref="B7:B13" si="0">SUM(B8)</f>
+        <v>7</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -10347,8 +10347,8 @@
         <v>139</v>
       </c>
       <c r="B10" s="35">
-        <f>SUM(B9)</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -10362,8 +10362,8 @@
         <v>140</v>
       </c>
       <c r="B11" s="35">
-        <f>SUM(B10)</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -10377,8 +10377,8 @@
         <v>141</v>
       </c>
       <c r="B12" s="35">
-        <f>SUM(B11)</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -10392,8 +10392,8 @@
         <v>142</v>
       </c>
       <c r="B13" s="35">
-        <f>SUM(B12)</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -10458,7 +10458,7 @@
         <v>276</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -10481,7 +10481,7 @@
         <v>277</v>
       </c>
       <c r="G22" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -10550,7 +10550,7 @@
         <v>282</v>
       </c>
       <c r="G25" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="H25" t="s">
         <v>278</v>
@@ -10668,7 +10668,7 @@
         <v>287</v>
       </c>
       <c r="G30" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -10691,7 +10691,7 @@
         <v>288</v>
       </c>
       <c r="G31" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -10699,7 +10699,7 @@
         <v>0</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:B55" si="0">B6</f>
+        <f t="shared" ref="B48:B55" si="1">B6</f>
         <v>11</v>
       </c>
     </row>
@@ -10708,8 +10708,8 @@
         <v>1</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -10717,8 +10717,8 @@
         <v>2</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -10726,8 +10726,8 @@
         <v>3</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -10735,8 +10735,8 @@
         <v>4</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -10744,8 +10744,8 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -10753,8 +10753,8 @@
         <v>6</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -10762,8 +10762,8 @@
         <v>7</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
In the Customer class, I have added defined the == and != operators for comparing customers. I have also created a new class, Sales_Associate, and have updated Shop to store them as well. Finally, main.cpp has a fully functional Customer_Dialog and Sales_Associate_Dialog, which prompt the user for information to create new Customers and Sales Associates, respectively.
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -4784,25 +4784,25 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11456,8 +11456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11557,8 +11557,8 @@
         <v>136</v>
       </c>
       <c r="B7" s="35">
-        <f>SUM(B6, -2)</f>
-        <v>25</v>
+        <f>SUM(B6, -4)</f>
+        <v>23</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -11573,7 +11573,7 @@
       </c>
       <c r="B8" s="35">
         <f>SUM(B7)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -11588,7 +11588,7 @@
       </c>
       <c r="B9" s="35">
         <f t="shared" ref="B9:B11" si="0">SUM(B8)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -11603,7 +11603,7 @@
       </c>
       <c r="B10" s="35">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -11618,7 +11618,7 @@
       </c>
       <c r="B11" s="35">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -11633,7 +11633,7 @@
       </c>
       <c r="B12" s="35">
         <f>SUM(B11)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -11648,7 +11648,7 @@
       </c>
       <c r="B13" s="35">
         <f>SUM(B12)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -11759,7 +11759,7 @@
         <v>288</v>
       </c>
       <c r="G23" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -11782,7 +11782,7 @@
         <v>289</v>
       </c>
       <c r="G24" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -12338,7 +12338,7 @@
       </c>
       <c r="B60">
         <f>B7</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -12347,7 +12347,7 @@
       </c>
       <c r="B61">
         <f>B8</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -12356,7 +12356,7 @@
       </c>
       <c r="B62">
         <f>B9</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -12365,7 +12365,7 @@
       </c>
       <c r="B63">
         <f>B10</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -12374,7 +12374,7 @@
       </c>
       <c r="B64">
         <f>B11</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="B65">
         <f>B12</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -12392,7 +12392,7 @@
       </c>
       <c r="B66">
         <f>B13</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the robot order dialog. Also added debug options to create random customers and sales associates
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="315">
   <si>
     <t>Product Name:</t>
   </si>
@@ -899,9 +899,6 @@
     <t>Create an Address class that stores a street address</t>
   </si>
   <si>
-    <t>Create a Beloved Customer class</t>
-  </si>
-  <si>
     <t>Add a dialog to create a new beloved customer</t>
   </si>
   <si>
@@ -911,39 +908,24 @@
     <t>Add menu option to create a new customer</t>
   </si>
   <si>
-    <t>Create &gt; Customer</t>
-  </si>
-  <si>
     <t>Add functions/callbacks that will extract the information from the customer dialog</t>
   </si>
   <si>
-    <t>Create a Sales Associate class</t>
-  </si>
-  <si>
     <t>Add a dialog to create a new sales associate</t>
   </si>
   <si>
     <t>Add menu option to create a new sales associate</t>
   </si>
   <si>
-    <t>Create &gt; Sales Associate</t>
-  </si>
-  <si>
     <t>Add functions/callbacks that will extract the information from the sales associate dialog</t>
   </si>
   <si>
-    <t>Create a Robot Order class</t>
-  </si>
-  <si>
     <t>Add a dialog to create a new robot order</t>
   </si>
   <si>
     <t>Add menu option to create a new robot order</t>
   </si>
   <si>
-    <t>Create &gt; Robot Order</t>
-  </si>
-  <si>
     <t>Add function/callbacks that will extract the information from the order dialog</t>
   </si>
   <si>
@@ -968,13 +950,31 @@
     <t>Update UML diagrams</t>
   </si>
   <si>
-    <t>Update the user manual</t>
-  </si>
-  <si>
     <t>Update sales brochure</t>
   </si>
   <si>
     <t>Proofread sales brochure</t>
+  </si>
+  <si>
+    <t>Create a Customer class and update the Shop class accordingly</t>
+  </si>
+  <si>
+    <t>Create a Sales Associate class and update the Shop class accordingly</t>
+  </si>
+  <si>
+    <t>Create a Robot Order class and update the Shop class accordingly</t>
+  </si>
+  <si>
+    <t>New &gt; Customer</t>
+  </si>
+  <si>
+    <t>New &gt; Sales Associate</t>
+  </si>
+  <si>
+    <t>New &gt; Robot Order</t>
+  </si>
+  <si>
+    <t>Redo the user manual</t>
   </si>
 </sst>
 </file>
@@ -4743,10 +4743,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sprint 8 Backlog'!$A$59:$A$66</c:f>
+              <c:f>'Sprint 8 Backlog'!$A$59:$A$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4764,45 +4764,33 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sprint 8 Backlog'!$B$59:$B$66</c:f>
+              <c:f>'Sprint 8 Backlog'!$B$59:$B$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4829,7 +4817,7 @@
         <c:axId val="393249400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
+          <c:max val="5"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -11454,10 +11442,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11557,8 +11545,8 @@
         <v>136</v>
       </c>
       <c r="B7" s="35">
-        <f>SUM(B6, -4)</f>
-        <v>23</v>
+        <f>SUM(B6)</f>
+        <v>27</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -11572,7 +11560,7 @@
         <v>137</v>
       </c>
       <c r="B8" s="35">
-        <f>SUM(B7)</f>
+        <f>SUM(B7, -4)</f>
         <v>23</v>
       </c>
       <c r="C8" s="29"/>
@@ -11587,8 +11575,8 @@
         <v>138</v>
       </c>
       <c r="B9" s="35">
-        <f t="shared" ref="B9:B11" si="0">SUM(B8)</f>
-        <v>23</v>
+        <f>SUM(B8, -9)</f>
+        <v>14</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -11602,8 +11590,8 @@
         <v>139</v>
       </c>
       <c r="B10" s="35">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f t="shared" ref="B10:B11" si="0">SUM(B9)</f>
+        <v>14</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -11618,7 +11606,7 @@
       </c>
       <c r="B11" s="35">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -11628,34 +11616,20 @@
       <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="35">
-        <f>SUM(B11)</f>
-        <v>23</v>
-      </c>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="35">
-        <f>SUM(B12)</f>
-        <v>23</v>
-      </c>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
@@ -11779,7 +11753,7 @@
         <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="G24" t="s">
         <v>170</v>
@@ -11802,10 +11776,10 @@
         <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G25" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -11813,7 +11787,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s">
         <v>152</v>
@@ -11825,13 +11799,13 @@
         <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G26" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="H26" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -11839,7 +11813,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C27" t="s">
         <v>152</v>
@@ -11851,10 +11825,10 @@
         <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G27" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -11874,10 +11848,10 @@
         <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="G28" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -11897,10 +11871,10 @@
         <v>150</v>
       </c>
       <c r="F29" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G29" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -11920,13 +11894,13 @@
         <v>150</v>
       </c>
       <c r="F30" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G30" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="H30" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
@@ -11946,10 +11920,10 @@
         <v>150</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G31" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -11969,10 +11943,10 @@
         <v>150</v>
       </c>
       <c r="F32" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="G32" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -11992,10 +11966,10 @@
         <v>150</v>
       </c>
       <c r="F33" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G33" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -12015,13 +11989,13 @@
         <v>150</v>
       </c>
       <c r="F34" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="G34" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="H34" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -12041,10 +12015,10 @@
         <v>150</v>
       </c>
       <c r="F35" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G35" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
@@ -12064,7 +12038,7 @@
         <v>150</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G36" t="s">
         <v>148</v>
@@ -12087,7 +12061,7 @@
         <v>150</v>
       </c>
       <c r="F37" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G37" t="s">
         <v>148</v>
@@ -12110,7 +12084,7 @@
         <v>150</v>
       </c>
       <c r="F38" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G38" t="s">
         <v>148</v>
@@ -12133,7 +12107,7 @@
         <v>150</v>
       </c>
       <c r="F39" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G39" t="s">
         <v>148</v>
@@ -12156,7 +12130,7 @@
         <v>150</v>
       </c>
       <c r="F40" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G40" t="s">
         <v>148</v>
@@ -12179,7 +12153,7 @@
         <v>150</v>
       </c>
       <c r="F41" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G41" t="s">
         <v>148</v>
@@ -12202,7 +12176,7 @@
         <v>150</v>
       </c>
       <c r="F42" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="G42" t="s">
         <v>148</v>
@@ -12225,7 +12199,7 @@
         <v>150</v>
       </c>
       <c r="F43" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G43" t="s">
         <v>148</v>
@@ -12271,7 +12245,7 @@
         <v>150</v>
       </c>
       <c r="F45" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="G45" t="s">
         <v>148</v>
@@ -12294,7 +12268,7 @@
         <v>150</v>
       </c>
       <c r="F46" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G46" t="s">
         <v>148</v>
@@ -12328,7 +12302,7 @@
         <v>0</v>
       </c>
       <c r="B59">
-        <f>B6</f>
+        <f t="shared" ref="B59:B64" si="1">B6</f>
         <v>27</v>
       </c>
     </row>
@@ -12337,8 +12311,8 @@
         <v>1</v>
       </c>
       <c r="B60">
-        <f>B7</f>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -12346,7 +12320,7 @@
         <v>2</v>
       </c>
       <c r="B61">
-        <f>B8</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
@@ -12355,8 +12329,8 @@
         <v>3</v>
       </c>
       <c r="B62">
-        <f>B9</f>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -12364,8 +12338,8 @@
         <v>4</v>
       </c>
       <c r="B63">
-        <f>B10</f>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -12373,26 +12347,8 @@
         <v>5</v>
       </c>
       <c r="B64">
-        <f>B11</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>6</v>
-      </c>
-      <c r="B65">
-        <f>B12</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>7</v>
-      </c>
-      <c r="B66">
-        <f>B13</f>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>